<commit_message>
changes to chapter 2
</commit_message>
<xml_diff>
--- a/ch-2.xlsx
+++ b/ch-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George Mount\Documents\GitHub\hf-da-resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\hf-da-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62AF4D2-DEA7-443A-9E77-1B1CD7439B97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BEBED7-F279-482D-9499-49BCB3EE2C84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{41FF17D3-6413-44E5-8BED-7F783257B4DD}"/>
+    <workbookView xWindow="-25693" yWindow="-13" windowWidth="25786" windowHeight="14586" xr2:uid="{41FF17D3-6413-44E5-8BED-7F783257B4DD}"/>
   </bookViews>
   <sheets>
     <sheet name="orders" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="18">
   <si>
     <t>order_id</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>grande</t>
-  </si>
-  <si>
-    <t>customer_id</t>
   </si>
   <si>
     <t>state</t>
@@ -99,10 +96,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,13 +134,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{B3FF2DA4-1E14-49D5-83CC-833926D83822}"/>
   </tableStyles>
@@ -150,17 +161,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B0F0623-D17D-4213-A343-5D615902F6F2}" name="Table1" displayName="Table1" ref="A1:G17" totalsRowShown="0">
-  <autoFilter ref="A1:G17" xr:uid="{5F9373DA-C9AC-4444-9ABC-E320C6F850B3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="A1:A17"/>
-  </sortState>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{98777A29-1DC9-4BCB-870F-EF77A840A885}" name="customer_id"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B0F0623-D17D-4213-A343-5D615902F6F2}" name="Table1" displayName="Table1" ref="A1:F17" totalsRowShown="0">
+  <tableColumns count="6">
     <tableColumn id="7" xr3:uid="{94708CB3-7B0A-4652-99CB-90565D52C27B}" name="order_id"/>
     <tableColumn id="2" xr3:uid="{EBA12C1C-18FF-4598-9F93-B508D2B4D6F8}" name="beverage"/>
     <tableColumn id="3" xr3:uid="{345C6C2F-D44B-4EC6-AB39-7423A5C16864}" name="size"/>
-    <tableColumn id="4" xr3:uid="{65532DB2-3DDD-4263-98A3-26B09D61638D}" name="price"/>
+    <tableColumn id="4" xr3:uid="{65532DB2-3DDD-4263-98A3-26B09D61638D}" name="price" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{8DA25AD8-C370-44F7-89F5-2CC6F67F8689}" name="units"/>
     <tableColumn id="6" xr3:uid="{3BC8FDBF-5E0F-4D94-8CA3-4DEB1F160844}" name="pickup_or_delivery"/>
   </tableColumns>
@@ -480,418 +486,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E9AEAD-6085-4AAA-9C7F-A339D7BD2B4D}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.90625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.73828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.2578125" customWidth="1"/>
+    <col min="4" max="4" width="7.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.0703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.3671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A2">
+        <v>779545</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>617883</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.3793800000000012</v>
+      </c>
+      <c r="E3">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A4">
+        <v>701398</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.95</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A5">
+        <v>406505</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A6">
+        <v>181195</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.3793800000000012</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A7">
+        <v>751064</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.6644800000000002</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A8">
+        <v>661530</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A9">
+        <v>755787</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.6644800000000002</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A10">
+        <v>626864</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.6644800000000002</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A11">
+        <v>226085</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A12">
+        <v>263599</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A13">
+        <v>421973</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.379</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A14">
+        <v>386755</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.6644800000000002</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A15">
+        <v>807872</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>208</v>
-      </c>
-      <c r="B2">
-        <v>779545</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>4.8</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>253</v>
-      </c>
-      <c r="B3">
-        <v>617883</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>6.3793800000000012</v>
-      </c>
-      <c r="F3">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A16">
+        <v>479281</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>414</v>
-      </c>
-      <c r="B4">
-        <v>701398</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>3.95</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>414</v>
-      </c>
-      <c r="B5">
-        <v>406505</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="A17">
+        <v>360621</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>4.05</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>497</v>
-      </c>
-      <c r="B6">
-        <v>181195</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6">
-        <v>6.3793800000000012</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>514</v>
-      </c>
-      <c r="B7">
-        <v>751064</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7">
-        <v>2.6644800000000002</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>555</v>
-      </c>
-      <c r="B8">
-        <v>661530</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>4.8</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>671</v>
-      </c>
-      <c r="B9">
-        <v>755787</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9">
-        <v>2.6644800000000002</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>671</v>
-      </c>
-      <c r="B10">
-        <v>626864</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>2.6644800000000002</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>768</v>
-      </c>
-      <c r="B11">
-        <v>226085</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>1.95</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>813</v>
-      </c>
-      <c r="B12">
-        <v>263599</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>2.5</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>903</v>
-      </c>
-      <c r="B13">
-        <v>421973</v>
-      </c>
-      <c r="C13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="E13">
-        <v>2.379</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>918</v>
-      </c>
-      <c r="B14">
-        <v>386755</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14">
-        <v>2.6644800000000002</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>951</v>
-      </c>
-      <c r="B15">
-        <v>807872</v>
-      </c>
-      <c r="C15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>978</v>
-      </c>
-      <c r="B16">
-        <v>479281</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16">
-        <v>2.9</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>979</v>
-      </c>
-      <c r="B17">
-        <v>360621</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
+      <c r="D17" s="1">
+        <v>4.45</v>
       </c>
       <c r="E17">
-        <v>4.45</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -904,11 +860,11 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -924,14 +880,14 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.90625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13.88671875" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" customWidth="1"/>
+    <col min="2" max="2" width="19.73828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.8125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -951,7 +907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>661530</v>
       </c>
@@ -971,7 +927,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>263599</v>
       </c>
@@ -991,7 +947,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>755787</v>
       </c>
@@ -1011,7 +967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5">
         <v>181195</v>
       </c>
@@ -1031,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6">
         <v>807872</v>
       </c>
@@ -1051,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7">
         <v>226085</v>
       </c>
@@ -1071,7 +1027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8">
         <v>779545</v>
       </c>
@@ -1091,7 +1047,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9">
         <v>751064</v>
       </c>
@@ -1111,7 +1067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10">
         <v>626864</v>
       </c>
@@ -1131,7 +1087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>386755</v>
       </c>
@@ -1151,7 +1107,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A12">
         <v>479281</v>
       </c>
@@ -1171,7 +1127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A13">
         <v>406505</v>
       </c>
@@ -1191,7 +1147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A14">
         <v>421973</v>
       </c>
@@ -1211,7 +1167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A15">
         <v>617883</v>
       </c>
@@ -1231,7 +1187,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A16">
         <v>701398</v>
       </c>
@@ -1251,7 +1207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A17">
         <v>360621</v>
       </c>

</xml_diff>